<commit_message>
SGgripper Lengthend SGconnector Made guides more rigid Increased axle outer distance Loosend up connections
SGbracket
 screw length adjusted

XLS database
changed sm40 cable gap value
</commit_message>
<xml_diff>
--- a/Servos.xlsx
+++ b/Servos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Studium\Masterarbeit\GITHUB\SGcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5681794A-B24B-45D1-A232-9D1AD61D93AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA162463-33D3-49B8-84CF-A17D46C39555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{F8F14A97-BE2A-4D42-9DDF-16D4435D337E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F8F14A97-BE2A-4D42-9DDF-16D4435D337E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>[-22.25,-15.50;22.25,-15.5;22.25,-0.5;-22.25,-0.5]</t>
   </si>
   <si>
-    <t>[-22.25,-10;22.25,-10;22.25,10;-22.25,10]</t>
-  </si>
-  <si>
     <t>cable_gap_width</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>[17.5,0;-17.5,0;17.5,35;-17.5,35;17.5,-35;-17.5,-35]</t>
+  </si>
+  <si>
+    <t>[-22.25,-5;22.25,-5;22.25,15;-22.25,15]</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,10 +586,10 @@
         <v>23</v>
       </c>
       <c r="V1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" t="s">
         <v>29</v>
-      </c>
-      <c r="W1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="Q2" t="s">
         <v>27</v>
@@ -710,10 +710,10 @@
         <v>55.6</v>
       </c>
       <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" t="s">
         <v>31</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>32</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -722,7 +722,7 @@
         <v>26</v>
       </c>
       <c r="T3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U3">
         <v>2</v>
@@ -781,7 +781,7 @@
         <v>72.599999999999994</v>
       </c>
       <c r="P4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q4" t="s">
         <v>26</v>
@@ -793,7 +793,7 @@
         <v>26</v>
       </c>
       <c r="T4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U4">
         <v>2</v>

</xml_diff>

<commit_message>
Updated SGrotatingattach for sm85bl
</commit_message>
<xml_diff>
--- a/Servos.xlsx
+++ b/Servos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Studium\Masterarbeit\GITHUB\SGcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA162463-33D3-49B8-84CF-A17D46C39555}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529F060E-8CB4-4689-9866-C6E9D336CF17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F8F14A97-BE2A-4D42-9DDF-16D4435D337E}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{F8F14A97-BE2A-4D42-9DDF-16D4435D337E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,6 @@
     <t>cable_gap</t>
   </si>
   <si>
-    <t>[-25,-17.5;25,-17.5;25,-2.5;-25,-2.5]</t>
-  </si>
-  <si>
     <t>[-27,-22.5;27,-22.5;27,-7.5;-27,-7.5]</t>
   </si>
   <si>
@@ -140,7 +137,10 @@
     <t>[17.5,0;-17.5,0;17.5,35;-17.5,35;17.5,-35;-17.5,-35]</t>
   </si>
   <si>
-    <t>[-22.25,-5;22.25,-5;22.25,15;-22.25,15]</t>
+    <t>[-22.25,-2.5;22.25,-2.5;22.25,12.5;-22.25,12.5]</t>
+  </si>
+  <si>
+    <t>[-25,-7.5;25,-7.5;25,7.5;-25,7.5]</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +639,7 @@
         <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q2" t="s">
         <v>27</v>
@@ -710,10 +710,10 @@
         <v>55.6</v>
       </c>
       <c r="P3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" t="s">
         <v>30</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>31</v>
       </c>
       <c r="R3" t="s">
         <v>26</v>
@@ -722,7 +722,7 @@
         <v>26</v>
       </c>
       <c r="T3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U3">
         <v>2</v>
@@ -781,7 +781,7 @@
         <v>72.599999999999994</v>
       </c>
       <c r="P4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q4" t="s">
         <v>26</v>
@@ -793,7 +793,7 @@
         <v>26</v>
       </c>
       <c r="T4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U4">
         <v>2</v>

</xml_diff>

<commit_message>
SGLCLzdof Screw Holes for sm40bl
SGrotatinglockadapter
Compatible with sgbracket and SGrotatingdisk
</commit_message>
<xml_diff>
--- a/Servos.xlsx
+++ b/Servos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Studium\Masterarbeit\GITHUB\SGcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529F060E-8CB4-4689-9866-C6E9D336CF17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEE0C94-CD1C-412D-920C-DE8A53D24C8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{F8F14A97-BE2A-4D42-9DDF-16D4435D337E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F8F14A97-BE2A-4D42-9DDF-16D4435D337E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -110,15 +110,9 @@
     <t>[-8,6;8,6;-8,-6;8,-6]</t>
   </si>
   <si>
-    <t>[6,-16;-6,-16;-6,8]</t>
-  </si>
-  <si>
     <t>NaN</t>
   </si>
   <si>
-    <t>[-22.25,-15.50;22.25,-15.5;22.25,-0.5;-22.25,-0.5]</t>
-  </si>
-  <si>
     <t>cable_gap_width</t>
   </si>
   <si>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t>[-25,-7.5;25,-7.5;25,7.5;-25,7.5]</t>
+  </si>
+  <si>
+    <t>[-22.25,-15.5;22.25,-15.5;22.25,-3;-22.25,-3]</t>
+  </si>
+  <si>
+    <t>[6,-16;-6,-16;6,8]</t>
   </si>
 </sst>
 </file>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED0103E-A602-4AD3-ABE5-C65CF2A52130}">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,10 +586,10 @@
         <v>23</v>
       </c>
       <c r="V1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="W1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -639,19 +639,19 @@
         <v>42</v>
       </c>
       <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
         <v>34</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>27</v>
       </c>
       <c r="R2" t="s">
         <v>24</v>
       </c>
       <c r="S2" t="s">
+        <v>35</v>
+      </c>
+      <c r="T2" t="s">
         <v>25</v>
-      </c>
-      <c r="T2" t="s">
-        <v>26</v>
       </c>
       <c r="U2" s="1">
         <v>1.5</v>
@@ -660,7 +660,7 @@
         <v>20</v>
       </c>
       <c r="W2">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -710,19 +710,19 @@
         <v>55.6</v>
       </c>
       <c r="P3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="U3">
         <v>2</v>
@@ -731,7 +731,7 @@
         <v>20</v>
       </c>
       <c r="W3">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -781,19 +781,19 @@
         <v>72.599999999999994</v>
       </c>
       <c r="P4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="U4">
         <v>2</v>
@@ -802,10 +802,11 @@
         <v>20</v>
       </c>
       <c r="W4">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Streamlined Adapter functions into SGconnAdaptersLCL
</commit_message>
<xml_diff>
--- a/Servos.xlsx
+++ b/Servos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Studium\Masterarbeit\GITHUB\SGcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEE0C94-CD1C-412D-920C-DE8A53D24C8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F65487-CB29-4029-B5C4-EB6B600A252C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F8F14A97-BE2A-4D42-9DDF-16D4435D337E}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>cable_gap</t>
   </si>
   <si>
-    <t>[-27,-22.5;27,-22.5;27,-7.5;-27,-7.5]</t>
-  </si>
-  <si>
     <t>[14,0;-14,0;14,28;-14,28;14,-28;-14,-28]</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>[6,-16;-6,-16;6,8]</t>
+  </si>
+  <si>
+    <t>[-27,-15;27,-15;27,5;-27,5]</t>
   </si>
 </sst>
 </file>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED0103E-A602-4AD3-ABE5-C65CF2A52130}">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,16 +639,16 @@
         <v>42</v>
       </c>
       <c r="P2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R2" t="s">
         <v>24</v>
       </c>
       <c r="S2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T2" t="s">
         <v>25</v>
@@ -710,10 +710,10 @@
         <v>55.6</v>
       </c>
       <c r="P3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="R3" t="s">
         <v>25</v>
@@ -722,7 +722,7 @@
         <v>25</v>
       </c>
       <c r="T3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U3">
         <v>2</v>
@@ -781,7 +781,7 @@
         <v>72.599999999999994</v>
       </c>
       <c r="P4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q4" t="s">
         <v>25</v>
@@ -793,7 +793,7 @@
         <v>25</v>
       </c>
       <c r="T4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U4">
         <v>2</v>

</xml_diff>

<commit_message>
Updates before database adjustments
</commit_message>
<xml_diff>
--- a/Servos.xlsx
+++ b/Servos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Studium\Masterarbeit\GITHUB\SGcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A43907A-5D9C-4BCE-AF6A-AC9A8925817F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC900F23-95C5-455E-ADBA-42AA45502C77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F8F14A97-BE2A-4D42-9DDF-16D4435D337E}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{F8F14A97-BE2A-4D42-9DDF-16D4435D337E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,19 +512,19 @@
     <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
     <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="33" customWidth="1"/>
+    <col min="23" max="23" width="19" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Update Files to match new naming scheme in database
</commit_message>
<xml_diff>
--- a/Servos.xlsx
+++ b/Servos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_Studium\Masterarbeit\GITHUB\SGcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC900F23-95C5-455E-ADBA-42AA45502C77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EAE4F2-1E2D-4921-BEE7-9CFA917EBC53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{F8F14A97-BE2A-4D42-9DDF-16D4435D337E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{F8F14A97-BE2A-4D42-9DDF-16D4435D337E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>sm40bl</t>
   </si>
@@ -62,27 +62,6 @@
     <t>mounting_screw_R</t>
   </si>
   <si>
-    <t>screw_R</t>
-  </si>
-  <si>
-    <t>screw_f_hor_dis</t>
-  </si>
-  <si>
-    <t>screw_f_ver_dis</t>
-  </si>
-  <si>
-    <t>mount_screw_R</t>
-  </si>
-  <si>
-    <t>attach_top_R</t>
-  </si>
-  <si>
-    <t>attach_top_H</t>
-  </si>
-  <si>
-    <t>mount_screw_Num</t>
-  </si>
-  <si>
     <t>connect_R</t>
   </si>
   <si>
@@ -104,9 +83,6 @@
     <t>screw_mount_z</t>
   </si>
   <si>
-    <t>attach_screw_R</t>
-  </si>
-  <si>
     <t>[-8,6;8,6;-8,-6;8,-6]</t>
   </si>
   <si>
@@ -146,7 +122,25 @@
     <t>shaft_R</t>
   </si>
   <si>
-    <t>attach_screw_depth</t>
+    <t>connect_screw_R</t>
+  </si>
+  <si>
+    <t>connect_screw_circle_R</t>
+  </si>
+  <si>
+    <t>connect_top_R</t>
+  </si>
+  <si>
+    <t>connect_top_H</t>
+  </si>
+  <si>
+    <t>connect_screw_Num</t>
+  </si>
+  <si>
+    <t>connect_screw_depth</t>
+  </si>
+  <si>
+    <t>mounting_screw_depth</t>
   </si>
 </sst>
 </file>
@@ -499,36 +493,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED0103E-A602-4AD3-ABE5-C65CF2A52130}">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -542,70 +534,64 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" t="s">
-        <v>37</v>
-      </c>
-      <c r="X1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -625,64 +611,58 @@
         <v>11.25</v>
       </c>
       <c r="G2">
-        <v>1.5</v>
+        <v>11</v>
       </c>
       <c r="H2">
+        <v>4.5</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
         <v>2</v>
-      </c>
-      <c r="I2">
-        <v>16</v>
-      </c>
-      <c r="J2">
-        <v>12</v>
       </c>
       <c r="K2">
         <v>7</v>
       </c>
-      <c r="L2">
-        <v>4.5</v>
+      <c r="L2" s="1">
+        <v>2.5</v>
       </c>
       <c r="M2">
         <v>4</v>
       </c>
       <c r="N2">
-        <v>4</v>
-      </c>
-      <c r="O2">
-        <v>11</v>
-      </c>
-      <c r="P2">
         <v>42</v>
       </c>
-      <c r="Q2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" t="s">
-        <v>33</v>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2">
+        <v>1.5</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
       </c>
       <c r="S2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="T2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="U2" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2" s="1">
-        <v>1.5</v>
+        <v>17</v>
+      </c>
+      <c r="V2">
+        <v>20</v>
       </c>
       <c r="W2">
-        <v>3</v>
-      </c>
-      <c r="X2">
-        <v>20</v>
-      </c>
-      <c r="Y2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -702,64 +682,58 @@
         <v>15</v>
       </c>
       <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
         <v>2</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>28</v>
-      </c>
-      <c r="J3">
-        <v>28</v>
       </c>
       <c r="K3">
         <v>10.5</v>
       </c>
       <c r="L3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M3">
         <v>8</v>
       </c>
       <c r="N3">
+        <v>55.6</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" t="s">
+        <v>17</v>
+      </c>
+      <c r="U3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V3">
+        <v>20</v>
+      </c>
+      <c r="W3">
         <v>8</v>
       </c>
-      <c r="O3">
-        <v>13</v>
-      </c>
-      <c r="P3">
-        <v>55.6</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" t="s">
-        <v>25</v>
-      </c>
-      <c r="U3" t="s">
-        <v>28</v>
-      </c>
-      <c r="V3">
-        <v>2</v>
-      </c>
-      <c r="W3">
-        <v>3</v>
-      </c>
-      <c r="X3">
-        <v>20</v>
-      </c>
-      <c r="Y3">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -779,60 +753,54 @@
         <v>21.5</v>
       </c>
       <c r="G4">
+        <v>34</v>
+      </c>
+      <c r="H4">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>10</v>
+      </c>
+      <c r="J4">
         <v>2</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <v>35</v>
-      </c>
-      <c r="J4">
-        <v>35</v>
       </c>
       <c r="K4">
         <v>12.5</v>
       </c>
       <c r="L4">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="M4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N4">
-        <v>8</v>
-      </c>
-      <c r="O4">
-        <v>34</v>
-      </c>
-      <c r="P4">
         <v>72.599999999999994</v>
       </c>
-      <c r="Q4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" t="s">
-        <v>25</v>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>3</v>
       </c>
       <c r="S4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="T4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="U4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="V4">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="W4">
-        <v>3</v>
-      </c>
-      <c r="X4">
-        <v>20</v>
-      </c>
-      <c r="Y4">
         <v>8</v>
       </c>
     </row>

</xml_diff>